<commit_message>
added the September doc
</commit_message>
<xml_diff>
--- a/2024_09_housing_prices.xlsx
+++ b/2024_09_housing_prices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.khamidov\Documents\09_september\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B64825C-88C2-493F-8246-F49D4803634B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D062C02B-9988-4463-983D-6CA2C1890A79}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F0A68128-6003-4809-9CD7-322F14E0A5F8}"/>
+    <workbookView xWindow="11595" yWindow="2895" windowWidth="14385" windowHeight="11445" xr2:uid="{F0A68128-6003-4809-9CD7-322F14E0A5F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Регион_динамика_цен" sheetId="31" r:id="rId1"/>
@@ -1549,9 +1549,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="3" borderId="55" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="6" fillId="2" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1611,9 +1608,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="2" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="9" fillId="2" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1621,9 +1615,6 @@
     <xf numFmtId="167" fontId="6" fillId="3" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="6" fillId="3" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="6" fillId="3" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1656,9 +1647,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1827,6 +1815,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -2165,11 +2165,11 @@
   <dimension ref="A1:BJ31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="BF4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="BG4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D40" sqref="D40"/>
       <selection pane="topRight" activeCell="D40" sqref="D40"/>
       <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
-      <selection pane="bottomRight" activeCell="BM18" sqref="BM18"/>
+      <selection pane="bottomRight" activeCell="BH4" sqref="BH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2192,82 +2192,82 @@
   <sheetData>
     <row r="1" spans="1:62" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:62" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="219" t="s">
+      <c r="B2" s="215" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="220"/>
-      <c r="D2" s="226">
+      <c r="C2" s="216"/>
+      <c r="D2" s="222">
         <v>2022</v>
       </c>
-      <c r="E2" s="227"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
-      <c r="L2" s="228"/>
-      <c r="M2" s="228"/>
-      <c r="N2" s="228"/>
-      <c r="O2" s="229"/>
-      <c r="P2" s="230">
+      <c r="E2" s="223"/>
+      <c r="F2" s="224"/>
+      <c r="G2" s="224"/>
+      <c r="H2" s="224"/>
+      <c r="I2" s="224"/>
+      <c r="J2" s="224"/>
+      <c r="K2" s="224"/>
+      <c r="L2" s="224"/>
+      <c r="M2" s="224"/>
+      <c r="N2" s="224"/>
+      <c r="O2" s="225"/>
+      <c r="P2" s="226">
         <v>2023</v>
       </c>
-      <c r="Q2" s="231"/>
-      <c r="R2" s="231"/>
-      <c r="S2" s="231"/>
-      <c r="T2" s="231"/>
-      <c r="U2" s="231"/>
-      <c r="V2" s="231"/>
-      <c r="W2" s="231"/>
-      <c r="X2" s="231"/>
-      <c r="Y2" s="231"/>
-      <c r="Z2" s="231"/>
-      <c r="AA2" s="233"/>
-      <c r="AB2" s="230">
+      <c r="Q2" s="227"/>
+      <c r="R2" s="227"/>
+      <c r="S2" s="227"/>
+      <c r="T2" s="227"/>
+      <c r="U2" s="227"/>
+      <c r="V2" s="227"/>
+      <c r="W2" s="227"/>
+      <c r="X2" s="227"/>
+      <c r="Y2" s="227"/>
+      <c r="Z2" s="227"/>
+      <c r="AA2" s="229"/>
+      <c r="AB2" s="226">
         <v>2024</v>
       </c>
-      <c r="AC2" s="231"/>
-      <c r="AD2" s="231"/>
-      <c r="AE2" s="231"/>
-      <c r="AF2" s="233"/>
-      <c r="AG2" s="164"/>
-      <c r="AH2" s="164"/>
-      <c r="AI2" s="164"/>
-      <c r="AJ2" s="164"/>
-      <c r="AK2" s="230" t="s">
+      <c r="AC2" s="227"/>
+      <c r="AD2" s="227"/>
+      <c r="AE2" s="227"/>
+      <c r="AF2" s="229"/>
+      <c r="AG2" s="163"/>
+      <c r="AH2" s="163"/>
+      <c r="AI2" s="163"/>
+      <c r="AJ2" s="163"/>
+      <c r="AK2" s="226" t="s">
         <v>76</v>
       </c>
-      <c r="AL2" s="231"/>
-      <c r="AM2" s="231"/>
-      <c r="AN2" s="231"/>
-      <c r="AO2" s="231"/>
-      <c r="AP2" s="231"/>
-      <c r="AQ2" s="231"/>
-      <c r="AR2" s="231"/>
-      <c r="AS2" s="231"/>
-      <c r="AT2" s="232"/>
-      <c r="AU2" s="232"/>
-      <c r="AV2" s="232"/>
-      <c r="AW2" s="231"/>
-      <c r="AX2" s="233"/>
-      <c r="AY2" s="216" t="s">
+      <c r="AL2" s="227"/>
+      <c r="AM2" s="227"/>
+      <c r="AN2" s="227"/>
+      <c r="AO2" s="227"/>
+      <c r="AP2" s="227"/>
+      <c r="AQ2" s="227"/>
+      <c r="AR2" s="227"/>
+      <c r="AS2" s="227"/>
+      <c r="AT2" s="228"/>
+      <c r="AU2" s="228"/>
+      <c r="AV2" s="228"/>
+      <c r="AW2" s="227"/>
+      <c r="AX2" s="229"/>
+      <c r="AY2" s="212" t="s">
         <v>100</v>
       </c>
-      <c r="AZ2" s="217"/>
-      <c r="BA2" s="217"/>
-      <c r="BB2" s="217"/>
-      <c r="BC2" s="217"/>
-      <c r="BD2" s="217"/>
-      <c r="BE2" s="217"/>
-      <c r="BF2" s="217"/>
-      <c r="BG2" s="217"/>
-      <c r="BH2" s="217"/>
-      <c r="BI2" s="218"/>
+      <c r="AZ2" s="213"/>
+      <c r="BA2" s="213"/>
+      <c r="BB2" s="213"/>
+      <c r="BC2" s="213"/>
+      <c r="BD2" s="213"/>
+      <c r="BE2" s="213"/>
+      <c r="BF2" s="213"/>
+      <c r="BG2" s="213"/>
+      <c r="BH2" s="213"/>
+      <c r="BI2" s="214"/>
     </row>
     <row r="3" spans="1:62" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="221"/>
-      <c r="C3" s="222"/>
+      <c r="B3" s="217"/>
+      <c r="C3" s="218"/>
       <c r="D3" s="69" t="s">
         <v>0</v>
       </c>
@@ -2352,19 +2352,19 @@
       <c r="AE3" s="150" t="s">
         <v>87</v>
       </c>
-      <c r="AF3" s="169" t="s">
+      <c r="AF3" s="168" t="s">
         <v>89</v>
       </c>
-      <c r="AG3" s="172" t="s">
+      <c r="AG3" s="171" t="s">
         <v>90</v>
       </c>
-      <c r="AH3" s="201" t="s">
+      <c r="AH3" s="198" t="s">
         <v>91</v>
       </c>
-      <c r="AI3" s="205" t="s">
+      <c r="AI3" s="201" t="s">
         <v>92</v>
       </c>
-      <c r="AJ3" s="205" t="s">
+      <c r="AJ3" s="201" t="s">
         <v>94</v>
       </c>
       <c r="AK3" s="83" t="s">
@@ -2412,16 +2412,16 @@
       <c r="AY3" s="115" t="s">
         <v>97</v>
       </c>
-      <c r="AZ3" s="163" t="s">
+      <c r="AZ3" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="BA3" s="163" t="s">
+      <c r="BA3" s="162" t="s">
         <v>86</v>
       </c>
       <c r="BB3" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="BC3" s="168" t="s">
+      <c r="BC3" s="167" t="s">
         <v>89</v>
       </c>
       <c r="BD3" s="133" t="s">
@@ -2430,13 +2430,13 @@
       <c r="BE3" s="135" t="s">
         <v>91</v>
       </c>
-      <c r="BF3" s="163" t="s">
+      <c r="BF3" s="162" t="s">
         <v>92</v>
       </c>
-      <c r="BG3" s="163" t="s">
+      <c r="BG3" s="162" t="s">
         <v>94</v>
       </c>
-      <c r="BH3" s="202" t="s">
+      <c r="BH3" s="199" t="s">
         <v>103</v>
       </c>
       <c r="BI3" s="100" t="s">
@@ -2537,20 +2537,20 @@
       <c r="AE4" s="151">
         <v>545.45454545454504</v>
       </c>
-      <c r="AF4" s="170">
+      <c r="AF4" s="169">
         <v>571.42857142857144</v>
       </c>
-      <c r="AG4" s="200">
+      <c r="AG4" s="197">
         <v>541.47727272727252</v>
       </c>
       <c r="AH4" s="143">
         <v>543.51851851851802</v>
       </c>
-      <c r="AI4" s="197">
+      <c r="AI4" s="194">
         <v>562.5</v>
       </c>
-      <c r="AJ4" s="197">
-        <v>523.63636363636294</v>
+      <c r="AJ4" s="211">
+        <v>536</v>
       </c>
       <c r="AK4" s="87">
         <f t="shared" ref="AK4:AK17" si="0">+P4/O4-1</f>
@@ -2642,15 +2642,15 @@
       </c>
       <c r="BG4" s="119">
         <f t="shared" si="14"/>
-        <v>-6.9090909090910313E-2</v>
+        <v>-4.7111111111111104E-2</v>
       </c>
       <c r="BH4" s="119">
         <f>+AJ4/AA4-1</f>
-        <v>-3.6655052264809584E-2</v>
+        <v>-1.390940766550508E-2</v>
       </c>
       <c r="BI4" s="120">
         <f>+AJ4/X4-1</f>
-        <v>-1.2006861063466157E-2</v>
+        <v>1.132075471698113E-2</v>
       </c>
       <c r="BJ4" s="15"/>
     </row>
@@ -2748,19 +2748,19 @@
       <c r="AE5" s="151">
         <v>522.38805970149258</v>
       </c>
-      <c r="AF5" s="171">
+      <c r="AF5" s="170">
         <v>531.25</v>
       </c>
-      <c r="AG5" s="197">
+      <c r="AG5" s="194">
         <v>527.02922077922085</v>
       </c>
       <c r="AH5" s="143">
         <v>535.71428571428567</v>
       </c>
-      <c r="AI5" s="197">
+      <c r="AI5" s="194">
         <v>537.77777777777783</v>
       </c>
-      <c r="AJ5" s="197">
+      <c r="AJ5" s="194">
         <v>546.51162790697674</v>
       </c>
       <c r="AK5" s="44">
@@ -2959,19 +2959,19 @@
       <c r="AE6" s="151">
         <v>375</v>
       </c>
-      <c r="AF6" s="171">
+      <c r="AF6" s="170">
         <v>387.62755102040802</v>
       </c>
-      <c r="AG6" s="197">
+      <c r="AG6" s="194">
         <v>398.63013698630141</v>
       </c>
       <c r="AH6" s="143">
         <v>386.3095238095238</v>
       </c>
-      <c r="AI6" s="197">
+      <c r="AI6" s="194">
         <v>395.6521739130435</v>
       </c>
-      <c r="AJ6" s="197">
+      <c r="AJ6" s="194">
         <v>416.65277777777783</v>
       </c>
       <c r="AK6" s="44">
@@ -3170,19 +3170,19 @@
       <c r="AE7" s="151">
         <v>385.71428571428572</v>
       </c>
-      <c r="AF7" s="171">
+      <c r="AF7" s="170">
         <v>385.71428571428572</v>
       </c>
-      <c r="AG7" s="197">
+      <c r="AG7" s="194">
         <v>400</v>
       </c>
       <c r="AH7" s="143">
         <v>384.52380952380952</v>
       </c>
-      <c r="AI7" s="197">
+      <c r="AI7" s="194">
         <v>388.88888888888891</v>
       </c>
-      <c r="AJ7" s="197">
+      <c r="AJ7" s="194">
         <v>436.36363636363637</v>
       </c>
       <c r="AK7" s="44">
@@ -3381,19 +3381,19 @@
       <c r="AE8" s="151">
         <v>414.35923829130212</v>
       </c>
-      <c r="AF8" s="171">
+      <c r="AF8" s="170">
         <v>420.08530969376011</v>
       </c>
-      <c r="AG8" s="197">
+      <c r="AG8" s="194">
         <v>427.10615384615392</v>
       </c>
       <c r="AH8" s="143">
         <v>414.45277777777778</v>
       </c>
-      <c r="AI8" s="197">
+      <c r="AI8" s="194">
         <v>428.57142857142861</v>
       </c>
-      <c r="AJ8" s="197">
+      <c r="AJ8" s="194">
         <v>422.41379310344831</v>
       </c>
       <c r="AK8" s="44">
@@ -3592,19 +3592,19 @@
       <c r="AE9" s="151">
         <v>623.49920774647887</v>
       </c>
-      <c r="AF9" s="171">
+      <c r="AF9" s="170">
         <v>625.54411764705878</v>
       </c>
-      <c r="AG9" s="197">
+      <c r="AG9" s="194">
         <v>625.31578947368416</v>
       </c>
       <c r="AH9" s="143">
         <v>620</v>
       </c>
-      <c r="AI9" s="197">
+      <c r="AI9" s="194">
         <v>632.66</v>
       </c>
-      <c r="AJ9" s="197">
+      <c r="AJ9" s="194">
         <v>616.89814814814815</v>
       </c>
       <c r="AK9" s="44">
@@ -3803,19 +3803,19 @@
       <c r="AE10" s="151">
         <v>491.66666666666669</v>
       </c>
-      <c r="AF10" s="171">
+      <c r="AF10" s="170">
         <v>490.90909090909088</v>
       </c>
-      <c r="AG10" s="197">
+      <c r="AG10" s="194">
         <v>466.66666666666669</v>
       </c>
       <c r="AH10" s="143">
         <v>493.33333333333331</v>
       </c>
-      <c r="AI10" s="197">
+      <c r="AI10" s="194">
         <v>500</v>
       </c>
-      <c r="AJ10" s="197">
+      <c r="AJ10" s="194">
         <v>500</v>
       </c>
       <c r="AK10" s="44">
@@ -4014,19 +4014,19 @@
       <c r="AE11" s="151">
         <v>315.05309734513281</v>
       </c>
-      <c r="AF11" s="171">
+      <c r="AF11" s="170">
         <v>315.09333333333331</v>
       </c>
-      <c r="AG11" s="197">
+      <c r="AG11" s="194">
         <v>316.82020202020198</v>
       </c>
       <c r="AH11" s="143">
         <v>329.8</v>
       </c>
-      <c r="AI11" s="197">
+      <c r="AI11" s="194">
         <v>326.15194805194812</v>
       </c>
-      <c r="AJ11" s="197">
+      <c r="AJ11" s="194">
         <v>329.94</v>
       </c>
       <c r="AK11" s="44">
@@ -4225,19 +4225,19 @@
       <c r="AE12" s="151">
         <v>741.31631631631626</v>
       </c>
-      <c r="AF12" s="171">
+      <c r="AF12" s="170">
         <v>733.33333333333337</v>
       </c>
-      <c r="AG12" s="197">
+      <c r="AG12" s="194">
         <v>755.13626834381557</v>
       </c>
       <c r="AH12" s="143">
         <v>754.71698113207549</v>
       </c>
-      <c r="AI12" s="197">
+      <c r="AI12" s="194">
         <v>750</v>
       </c>
-      <c r="AJ12" s="197">
+      <c r="AJ12" s="194">
         <v>763.88888888888891</v>
       </c>
       <c r="AK12" s="44">
@@ -4436,19 +4436,19 @@
       <c r="AE13" s="151">
         <v>654.5454545454545</v>
       </c>
-      <c r="AF13" s="171">
+      <c r="AF13" s="170">
         <v>648.14814814814815</v>
       </c>
-      <c r="AG13" s="197">
+      <c r="AG13" s="194">
         <v>652.35814296241711</v>
       </c>
       <c r="AH13" s="143">
         <v>645.09569377990431</v>
       </c>
-      <c r="AI13" s="197">
+      <c r="AI13" s="194">
         <v>641.56545209176784</v>
       </c>
-      <c r="AJ13" s="197">
+      <c r="AJ13" s="194">
         <v>644.73684210526312</v>
       </c>
       <c r="AK13" s="44">
@@ -4647,19 +4647,19 @@
       <c r="AE14" s="151">
         <v>387.93103448275798</v>
       </c>
-      <c r="AF14" s="171">
+      <c r="AF14" s="170">
         <v>405.97413793103402</v>
       </c>
-      <c r="AG14" s="197">
+      <c r="AG14" s="194">
         <v>410.95890410958901</v>
       </c>
       <c r="AH14" s="143">
         <v>419</v>
       </c>
-      <c r="AI14" s="197">
+      <c r="AI14" s="194">
         <v>422.222222222222</v>
       </c>
-      <c r="AJ14" s="197">
+      <c r="AJ14" s="194">
         <v>431.506849315068</v>
       </c>
       <c r="AK14" s="44">
@@ -4858,19 +4858,19 @@
       <c r="AE15" s="151">
         <v>395.5625</v>
       </c>
-      <c r="AF15" s="171">
+      <c r="AF15" s="170">
         <v>423.07692307692309</v>
       </c>
-      <c r="AG15" s="197">
+      <c r="AG15" s="194">
         <v>423.38071428571419</v>
       </c>
       <c r="AH15" s="143">
         <v>437.5</v>
       </c>
-      <c r="AI15" s="197">
+      <c r="AI15" s="194">
         <v>422.67373063683311</v>
       </c>
-      <c r="AJ15" s="197">
+      <c r="AJ15" s="194">
         <v>437.1</v>
       </c>
       <c r="AK15" s="44">
@@ -5069,19 +5069,19 @@
       <c r="AE16" s="151">
         <v>428.57142857142861</v>
       </c>
-      <c r="AF16" s="171">
+      <c r="AF16" s="170">
         <v>419.67741935483872</v>
       </c>
-      <c r="AG16" s="197">
+      <c r="AG16" s="194">
         <v>431.0795454545455</v>
       </c>
       <c r="AH16" s="143">
         <v>436.80555555555549</v>
       </c>
-      <c r="AI16" s="197">
+      <c r="AI16" s="194">
         <v>439.09552845528458</v>
       </c>
-      <c r="AJ16" s="197">
+      <c r="AJ16" s="194">
         <v>425.531914893617</v>
       </c>
       <c r="AK16" s="44">
@@ -5277,22 +5277,22 @@
       <c r="AD17" s="114">
         <v>1142</v>
       </c>
-      <c r="AE17" s="171">
+      <c r="AE17" s="170">
         <v>1155</v>
       </c>
-      <c r="AF17" s="171">
+      <c r="AF17" s="170">
         <v>1155</v>
       </c>
-      <c r="AG17" s="197">
+      <c r="AG17" s="194">
         <v>1142</v>
       </c>
       <c r="AH17" s="141">
         <v>1126</v>
       </c>
-      <c r="AI17" s="197">
+      <c r="AI17" s="194">
         <v>1128</v>
       </c>
-      <c r="AJ17" s="215">
+      <c r="AJ17" s="211">
         <v>1117</v>
       </c>
       <c r="AK17" s="54">
@@ -5398,23 +5398,23 @@
       <c r="BJ17" s="15"/>
     </row>
     <row r="18" spans="1:62" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="223" t="s">
+      <c r="B18" s="219" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="224"/>
-      <c r="D18" s="225"/>
-      <c r="E18" s="225"/>
-      <c r="F18" s="225"/>
-      <c r="G18" s="225"/>
-      <c r="H18" s="225"/>
-      <c r="I18" s="225"/>
-      <c r="J18" s="225"/>
-      <c r="K18" s="225"/>
-      <c r="L18" s="225"/>
-      <c r="M18" s="225"/>
-      <c r="N18" s="225"/>
-      <c r="O18" s="225"/>
-      <c r="P18" s="225"/>
+      <c r="C18" s="220"/>
+      <c r="D18" s="221"/>
+      <c r="E18" s="221"/>
+      <c r="F18" s="221"/>
+      <c r="G18" s="221"/>
+      <c r="H18" s="221"/>
+      <c r="I18" s="221"/>
+      <c r="J18" s="221"/>
+      <c r="K18" s="221"/>
+      <c r="L18" s="221"/>
+      <c r="M18" s="221"/>
+      <c r="N18" s="221"/>
+      <c r="O18" s="221"/>
+      <c r="P18" s="221"/>
       <c r="Q18" s="14"/>
       <c r="R18" s="14"/>
       <c r="S18" s="14"/>
@@ -5426,15 +5426,15 @@
       <c r="Y18" s="14"/>
       <c r="Z18" s="14"/>
       <c r="AA18" s="14"/>
-      <c r="AB18" s="198"/>
+      <c r="AB18" s="195"/>
       <c r="AC18" s="14"/>
       <c r="AD18" s="14"/>
-      <c r="AE18" s="199"/>
-      <c r="AF18" s="199"/>
-      <c r="AG18" s="199"/>
-      <c r="AH18" s="199"/>
-      <c r="AI18" s="199"/>
-      <c r="AJ18" s="199"/>
+      <c r="AE18" s="196"/>
+      <c r="AF18" s="196"/>
+      <c r="AG18" s="196"/>
+      <c r="AH18" s="196"/>
+      <c r="AI18" s="196"/>
+      <c r="AJ18" s="196"/>
       <c r="AK18" s="76">
         <f>+AVERAGE(AK4:AK17)</f>
         <v>9.3962846348428462E-3</v>
@@ -5491,49 +5491,49 @@
         <f t="shared" ref="AX18:BC18" si="28">+AVERAGE(AX4:AX17)</f>
         <v>0.17260374482862359</v>
       </c>
-      <c r="AY18" s="165">
+      <c r="AY18" s="164">
         <f t="shared" si="28"/>
         <v>1.6167388710443899E-2</v>
       </c>
-      <c r="AZ18" s="166">
+      <c r="AZ18" s="165">
         <f t="shared" si="28"/>
         <v>8.1757886072734241E-3</v>
       </c>
-      <c r="BA18" s="166">
+      <c r="BA18" s="165">
         <f t="shared" si="28"/>
         <v>4.5160593251503834E-3</v>
       </c>
-      <c r="BB18" s="166">
+      <c r="BB18" s="165">
         <f t="shared" si="28"/>
         <v>-6.5735212880211656E-3</v>
       </c>
-      <c r="BC18" s="166">
+      <c r="BC18" s="165">
         <f t="shared" si="28"/>
         <v>1.3479737673764194E-2</v>
       </c>
-      <c r="BD18" s="166">
+      <c r="BD18" s="165">
         <f>+AVERAGE(BD4:BD17)</f>
         <v>3.0460018300039115E-3</v>
       </c>
-      <c r="BE18" s="166">
+      <c r="BE18" s="165">
         <f>+AVERAGE(BE4:BE17)</f>
         <v>3.6525996244977654E-3</v>
       </c>
-      <c r="BF18" s="166">
+      <c r="BF18" s="165">
         <f>+AVERAGE(BF4:BF17)</f>
         <v>7.1676182531904874E-3</v>
       </c>
-      <c r="BG18" s="166">
+      <c r="BG18" s="165">
         <f>+AVERAGE(BG4:BG17)</f>
-        <v>9.5414271235246817E-3</v>
-      </c>
-      <c r="BH18" s="166">
+        <v>1.1111412693510339E-2</v>
+      </c>
+      <c r="BH18" s="165">
         <f>+(1+AY18)*(1+AZ18)*(1+BB18)*(1+BA18)*(1+BC18)*(1+BD18)*(1+BE18)*(1+BF18)*(1+BG18)-1</f>
-        <v>6.0570070953833266E-2</v>
-      </c>
-      <c r="BI18" s="167">
+        <v>6.2219413578732397E-2</v>
+      </c>
+      <c r="BI18" s="166">
         <f>+AVERAGE(BI4:BI17)</f>
-        <v>7.5648385867919749E-2</v>
+        <v>7.731464413795168E-2</v>
       </c>
     </row>
     <row r="19" spans="1:62" ht="15" x14ac:dyDescent="0.2">
@@ -5603,7 +5603,7 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="AK4:AW17 AW20">
-    <cfRule type="dataBar" priority="44">
+    <cfRule type="dataBar" priority="45">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5617,7 +5617,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX4:AX17">
-    <cfRule type="dataBar" priority="43">
+    <cfRule type="dataBar" priority="44">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5631,6 +5631,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG4:BG17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BI4:BI18">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -5684,11 +5696,11 @@
   <dimension ref="A1:BI30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="BF2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D40" sqref="D40"/>
       <selection pane="topRight" activeCell="D40" sqref="D40"/>
       <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
-      <selection pane="bottomRight" activeCell="BG11" sqref="BG11"/>
+      <selection pane="bottomRight" activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5709,96 +5721,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
-      <c r="M1" s="240"/>
-      <c r="N1" s="240"/>
-      <c r="O1" s="240"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="236"/>
+      <c r="K1" s="236"/>
+      <c r="L1" s="236"/>
+      <c r="M1" s="236"/>
+      <c r="N1" s="236"/>
+      <c r="O1" s="236"/>
     </row>
     <row r="2" spans="1:61" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="240" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="245"/>
-      <c r="D2" s="241">
+      <c r="C2" s="241"/>
+      <c r="D2" s="237">
         <v>2022</v>
       </c>
-      <c r="E2" s="242"/>
-      <c r="F2" s="243"/>
-      <c r="G2" s="243"/>
-      <c r="H2" s="243"/>
-      <c r="I2" s="243"/>
-      <c r="J2" s="243"/>
-      <c r="K2" s="243"/>
-      <c r="L2" s="243"/>
-      <c r="M2" s="243"/>
-      <c r="N2" s="243"/>
-      <c r="O2" s="243"/>
-      <c r="P2" s="248">
+      <c r="E2" s="238"/>
+      <c r="F2" s="239"/>
+      <c r="G2" s="239"/>
+      <c r="H2" s="239"/>
+      <c r="I2" s="239"/>
+      <c r="J2" s="239"/>
+      <c r="K2" s="239"/>
+      <c r="L2" s="239"/>
+      <c r="M2" s="239"/>
+      <c r="N2" s="239"/>
+      <c r="O2" s="239"/>
+      <c r="P2" s="244">
         <v>2023</v>
       </c>
-      <c r="Q2" s="249"/>
-      <c r="R2" s="249"/>
-      <c r="S2" s="249"/>
-      <c r="T2" s="249"/>
-      <c r="U2" s="249"/>
-      <c r="V2" s="249"/>
-      <c r="W2" s="249"/>
-      <c r="X2" s="249"/>
-      <c r="Y2" s="249"/>
-      <c r="Z2" s="249"/>
-      <c r="AA2" s="249"/>
-      <c r="AB2" s="249">
+      <c r="Q2" s="245"/>
+      <c r="R2" s="245"/>
+      <c r="S2" s="245"/>
+      <c r="T2" s="245"/>
+      <c r="U2" s="245"/>
+      <c r="V2" s="245"/>
+      <c r="W2" s="245"/>
+      <c r="X2" s="245"/>
+      <c r="Y2" s="245"/>
+      <c r="Z2" s="245"/>
+      <c r="AA2" s="245"/>
+      <c r="AB2" s="245">
         <v>2024</v>
       </c>
-      <c r="AC2" s="249"/>
-      <c r="AD2" s="249"/>
-      <c r="AE2" s="249"/>
-      <c r="AF2" s="249"/>
-      <c r="AG2" s="173"/>
-      <c r="AH2" s="173"/>
-      <c r="AI2" s="173"/>
-      <c r="AJ2" s="173"/>
-      <c r="AK2" s="232" t="s">
+      <c r="AC2" s="245"/>
+      <c r="AD2" s="245"/>
+      <c r="AE2" s="245"/>
+      <c r="AF2" s="245"/>
+      <c r="AG2" s="172"/>
+      <c r="AH2" s="172"/>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="172"/>
+      <c r="AK2" s="228" t="s">
         <v>76</v>
       </c>
-      <c r="AL2" s="232"/>
-      <c r="AM2" s="232"/>
-      <c r="AN2" s="232"/>
-      <c r="AO2" s="232"/>
-      <c r="AP2" s="232"/>
-      <c r="AQ2" s="232"/>
-      <c r="AR2" s="232"/>
-      <c r="AS2" s="232"/>
-      <c r="AT2" s="232"/>
-      <c r="AU2" s="232"/>
-      <c r="AV2" s="232"/>
-      <c r="AW2" s="232"/>
-      <c r="AX2" s="237"/>
-      <c r="AY2" s="234" t="s">
+      <c r="AL2" s="228"/>
+      <c r="AM2" s="228"/>
+      <c r="AN2" s="228"/>
+      <c r="AO2" s="228"/>
+      <c r="AP2" s="228"/>
+      <c r="AQ2" s="228"/>
+      <c r="AR2" s="228"/>
+      <c r="AS2" s="228"/>
+      <c r="AT2" s="228"/>
+      <c r="AU2" s="228"/>
+      <c r="AV2" s="228"/>
+      <c r="AW2" s="228"/>
+      <c r="AX2" s="233"/>
+      <c r="AY2" s="230" t="s">
         <v>101</v>
       </c>
-      <c r="AZ2" s="235"/>
-      <c r="BA2" s="235"/>
-      <c r="BB2" s="235"/>
-      <c r="BC2" s="235"/>
-      <c r="BD2" s="235"/>
-      <c r="BE2" s="235"/>
-      <c r="BF2" s="235"/>
-      <c r="BG2" s="235"/>
-      <c r="BH2" s="235"/>
-      <c r="BI2" s="236"/>
+      <c r="AZ2" s="231"/>
+      <c r="BA2" s="231"/>
+      <c r="BB2" s="231"/>
+      <c r="BC2" s="231"/>
+      <c r="BD2" s="231"/>
+      <c r="BE2" s="231"/>
+      <c r="BF2" s="231"/>
+      <c r="BG2" s="231"/>
+      <c r="BH2" s="231"/>
+      <c r="BI2" s="232"/>
     </row>
     <row r="3" spans="1:61" s="7" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="246"/>
-      <c r="C3" s="247"/>
+      <c r="B3" s="242"/>
+      <c r="C3" s="243"/>
       <c r="D3" s="56" t="s">
         <v>0</v>
       </c>
@@ -5883,22 +5895,22 @@
       <c r="AE3" s="145" t="s">
         <v>87</v>
       </c>
-      <c r="AF3" s="177" t="s">
+      <c r="AF3" s="176" t="s">
         <v>89</v>
       </c>
-      <c r="AG3" s="179" t="s">
+      <c r="AG3" s="178" t="s">
         <v>90</v>
       </c>
-      <c r="AH3" s="179" t="s">
+      <c r="AH3" s="178" t="s">
         <v>91</v>
       </c>
-      <c r="AI3" s="179" t="s">
+      <c r="AI3" s="178" t="s">
         <v>92</v>
       </c>
-      <c r="AJ3" s="177" t="s">
+      <c r="AJ3" s="176" t="s">
         <v>94</v>
       </c>
-      <c r="AK3" s="177" t="s">
+      <c r="AK3" s="176" t="s">
         <v>0</v>
       </c>
       <c r="AL3" s="57" t="s">
@@ -6068,7 +6080,7 @@
       <c r="AE4" s="146">
         <v>964.91228070175441</v>
       </c>
-      <c r="AF4" s="174">
+      <c r="AF4" s="173">
         <v>969.44962686567169</v>
       </c>
       <c r="AG4" s="142">
@@ -6080,10 +6092,10 @@
       <c r="AI4" s="142">
         <v>941.66666666666674</v>
       </c>
-      <c r="AJ4" s="174">
+      <c r="AJ4" s="173">
         <v>933.33333333333337</v>
       </c>
-      <c r="AK4" s="212">
+      <c r="AK4" s="208">
         <f t="shared" ref="AK4:AK15" si="0">+P4/O4-1</f>
         <v>2.94460795752014E-2</v>
       </c>
@@ -6278,7 +6290,7 @@
       <c r="AE5" s="147">
         <v>979.69072164948454</v>
       </c>
-      <c r="AF5" s="175">
+      <c r="AF5" s="174">
         <v>972.19880576044966</v>
       </c>
       <c r="AG5" s="143">
@@ -6290,10 +6302,10 @@
       <c r="AI5" s="143">
         <v>941.66666666666663</v>
       </c>
-      <c r="AJ5" s="211">
+      <c r="AJ5" s="207">
         <v>923.61111111111109</v>
       </c>
-      <c r="AK5" s="213">
+      <c r="AK5" s="209">
         <f t="shared" si="0"/>
         <v>4.9930787150795908E-3</v>
       </c>
@@ -6488,7 +6500,7 @@
       <c r="AE6" s="147">
         <v>1105.2631578947371</v>
       </c>
-      <c r="AF6" s="175">
+      <c r="AF6" s="174">
         <v>1106.666666666667</v>
       </c>
       <c r="AG6" s="143">
@@ -6500,10 +6512,10 @@
       <c r="AI6" s="143">
         <v>1074.0740740740739</v>
       </c>
-      <c r="AJ6" s="211">
+      <c r="AJ6" s="207">
         <v>1060.30303030303</v>
       </c>
-      <c r="AK6" s="213">
+      <c r="AK6" s="209">
         <f t="shared" si="0"/>
         <v>1.9454545454545391E-2</v>
       </c>
@@ -6698,7 +6710,7 @@
       <c r="AE7" s="147">
         <v>1071.4285714285711</v>
       </c>
-      <c r="AF7" s="175">
+      <c r="AF7" s="174">
         <v>1071.4285714285711</v>
       </c>
       <c r="AG7" s="143">
@@ -6710,10 +6722,10 @@
       <c r="AI7" s="143">
         <v>1067.441860465116</v>
       </c>
-      <c r="AJ7" s="211">
+      <c r="AJ7" s="207">
         <v>1056.864375461937</v>
       </c>
-      <c r="AK7" s="213">
+      <c r="AK7" s="209">
         <f t="shared" si="0"/>
         <v>2.796052631578938E-2</v>
       </c>
@@ -6908,7 +6920,7 @@
       <c r="AE8" s="147">
         <v>1133.333333333333</v>
       </c>
-      <c r="AF8" s="175">
+      <c r="AF8" s="174">
         <v>1142.8571428571429</v>
       </c>
       <c r="AG8" s="143">
@@ -6920,10 +6932,10 @@
       <c r="AI8" s="143">
         <v>1102.7342500799491</v>
       </c>
-      <c r="AJ8" s="211">
+      <c r="AJ8" s="207">
         <v>1089.7435897435901</v>
       </c>
-      <c r="AK8" s="213">
+      <c r="AK8" s="209">
         <f t="shared" si="0"/>
         <v>1.4201701701701763E-2</v>
       </c>
@@ -7118,7 +7130,7 @@
       <c r="AE9" s="147">
         <v>1166.666666666667</v>
       </c>
-      <c r="AF9" s="175">
+      <c r="AF9" s="174">
         <v>1168.375</v>
       </c>
       <c r="AG9" s="143">
@@ -7130,10 +7142,10 @@
       <c r="AI9" s="143">
         <v>1145.833333333333</v>
       </c>
-      <c r="AJ9" s="211">
+      <c r="AJ9" s="207">
         <v>1117.9144385026741</v>
       </c>
-      <c r="AK9" s="213">
+      <c r="AK9" s="209">
         <f t="shared" si="0"/>
         <v>2.8945852534562277E-2</v>
       </c>
@@ -7328,7 +7340,7 @@
       <c r="AE10" s="147">
         <v>1229.864864864865</v>
       </c>
-      <c r="AF10" s="175">
+      <c r="AF10" s="174">
         <v>1247.5</v>
       </c>
       <c r="AG10" s="143">
@@ -7340,10 +7352,10 @@
       <c r="AI10" s="143">
         <v>1190.4761904761899</v>
       </c>
-      <c r="AJ10" s="211">
+      <c r="AJ10" s="207">
         <v>1184.2105263157889</v>
       </c>
-      <c r="AK10" s="213">
+      <c r="AK10" s="209">
         <f t="shared" si="0"/>
         <v>1.4285714285714013E-2</v>
       </c>
@@ -7538,7 +7550,7 @@
       <c r="AE11" s="147">
         <v>1200</v>
       </c>
-      <c r="AF11" s="175">
+      <c r="AF11" s="174">
         <v>1227.9873271889401</v>
       </c>
       <c r="AG11" s="143">
@@ -7550,10 +7562,10 @@
       <c r="AI11" s="143">
         <v>1199.2533333333331</v>
       </c>
-      <c r="AJ11" s="211">
+      <c r="AJ11" s="207">
         <v>1168.9655172413791</v>
       </c>
-      <c r="AK11" s="213">
+      <c r="AK11" s="209">
         <f t="shared" si="0"/>
         <v>2.4156239326853512E-3</v>
       </c>
@@ -7748,7 +7760,7 @@
       <c r="AE12" s="147">
         <v>1200</v>
       </c>
-      <c r="AF12" s="175">
+      <c r="AF12" s="174">
         <v>1190.4761904761899</v>
       </c>
       <c r="AG12" s="143">
@@ -7760,10 +7772,10 @@
       <c r="AI12" s="143">
         <v>1186.356589147287</v>
       </c>
-      <c r="AJ12" s="211">
+      <c r="AJ12" s="207">
         <v>1192.928039702233</v>
       </c>
-      <c r="AK12" s="213">
+      <c r="AK12" s="209">
         <f t="shared" si="0"/>
         <v>2.7432096597145961E-2</v>
       </c>
@@ -7958,7 +7970,7 @@
       <c r="AE13" s="147">
         <v>1328.5714285714289</v>
       </c>
-      <c r="AF13" s="175">
+      <c r="AF13" s="174">
         <v>1300</v>
       </c>
       <c r="AG13" s="143">
@@ -7970,10 +7982,10 @@
       <c r="AI13" s="143">
         <v>1287.2413793103451</v>
       </c>
-      <c r="AJ13" s="211">
+      <c r="AJ13" s="207">
         <v>1306.666666666667</v>
       </c>
-      <c r="AK13" s="213">
+      <c r="AK13" s="209">
         <f t="shared" si="0"/>
         <v>2.6432158293152597E-2</v>
       </c>
@@ -8168,7 +8180,7 @@
       <c r="AE14" s="148">
         <v>1322.418572418572</v>
       </c>
-      <c r="AF14" s="178">
+      <c r="AF14" s="177">
         <v>1307.1794871794871</v>
       </c>
       <c r="AG14" s="143">
@@ -8180,10 +8192,10 @@
       <c r="AI14" s="143">
         <v>1273.333333333333</v>
       </c>
-      <c r="AJ14" s="211">
+      <c r="AJ14" s="207">
         <v>1253.700564971751</v>
       </c>
-      <c r="AK14" s="213">
+      <c r="AK14" s="209">
         <f t="shared" si="0"/>
         <v>1.1297908745934837E-2</v>
       </c>
@@ -8285,10 +8297,10 @@
       </c>
     </row>
     <row r="15" spans="1:61" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="238" t="s">
+      <c r="B15" s="234" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="239"/>
+      <c r="C15" s="235"/>
       <c r="D15" s="38">
         <v>730.02347994203103</v>
       </c>
@@ -8373,23 +8385,23 @@
       <c r="AE15" s="149">
         <v>1155</v>
       </c>
-      <c r="AF15" s="176">
+      <c r="AF15" s="175">
         <v>1155</v>
       </c>
-      <c r="AG15" s="180">
+      <c r="AG15" s="179">
         <v>1142</v>
       </c>
-      <c r="AH15" s="180">
+      <c r="AH15" s="179">
         <v>1126</v>
       </c>
-      <c r="AI15" s="180">
+      <c r="AI15" s="179">
         <v>1128</v>
       </c>
-      <c r="AJ15" s="176">
+      <c r="AJ15" s="175">
         <f>AVERAGE(AJ4:AJ14)</f>
         <v>1117.1128357594084</v>
       </c>
-      <c r="AK15" s="214">
+      <c r="AK15" s="210">
         <f t="shared" si="0"/>
         <v>1.8675110953239704E-2</v>
       </c>
@@ -8678,21 +8690,20 @@
   <dimension ref="A1:BH15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AX14" sqref="AX14"/>
+      <pane xSplit="2" topLeftCell="BC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BH13" sqref="BH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="13" width="15.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="16" width="13.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="22" width="15.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="23" max="26" width="14" style="1" hidden="1" customWidth="1"/>
-    <col min="27" max="35" width="14" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
+    <col min="4" max="13" width="15.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="13.5703125" style="1" customWidth="1"/>
+    <col min="17" max="22" width="15.140625" style="1" customWidth="1"/>
+    <col min="23" max="35" width="14" style="1" customWidth="1"/>
     <col min="36" max="36" width="10" style="1" hidden="1" customWidth="1"/>
     <col min="37" max="39" width="11.5703125" style="1" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="12.7109375" style="1" hidden="1" customWidth="1"/>
@@ -8707,82 +8718,82 @@
   <sheetData>
     <row r="1" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:60" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="257" t="s">
+      <c r="A2" s="253" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="258"/>
-      <c r="C2" s="253">
+      <c r="B2" s="254"/>
+      <c r="C2" s="249">
         <v>2022</v>
       </c>
-      <c r="D2" s="254"/>
-      <c r="E2" s="255"/>
-      <c r="F2" s="255"/>
-      <c r="G2" s="255"/>
-      <c r="H2" s="255"/>
-      <c r="I2" s="255"/>
-      <c r="J2" s="255"/>
-      <c r="K2" s="255"/>
-      <c r="L2" s="255"/>
-      <c r="M2" s="255"/>
-      <c r="N2" s="256"/>
-      <c r="O2" s="263">
+      <c r="D2" s="250"/>
+      <c r="E2" s="251"/>
+      <c r="F2" s="251"/>
+      <c r="G2" s="251"/>
+      <c r="H2" s="251"/>
+      <c r="I2" s="251"/>
+      <c r="J2" s="251"/>
+      <c r="K2" s="251"/>
+      <c r="L2" s="251"/>
+      <c r="M2" s="251"/>
+      <c r="N2" s="252"/>
+      <c r="O2" s="259">
         <v>2023</v>
       </c>
-      <c r="P2" s="261"/>
-      <c r="Q2" s="261"/>
-      <c r="R2" s="261"/>
-      <c r="S2" s="261"/>
-      <c r="T2" s="261"/>
-      <c r="U2" s="261"/>
-      <c r="V2" s="261"/>
-      <c r="W2" s="261"/>
-      <c r="X2" s="261"/>
-      <c r="Y2" s="261"/>
-      <c r="Z2" s="262"/>
-      <c r="AA2" s="263">
+      <c r="P2" s="257"/>
+      <c r="Q2" s="257"/>
+      <c r="R2" s="257"/>
+      <c r="S2" s="257"/>
+      <c r="T2" s="257"/>
+      <c r="U2" s="257"/>
+      <c r="V2" s="257"/>
+      <c r="W2" s="257"/>
+      <c r="X2" s="257"/>
+      <c r="Y2" s="257"/>
+      <c r="Z2" s="258"/>
+      <c r="AA2" s="259">
         <v>2024</v>
       </c>
-      <c r="AB2" s="261"/>
-      <c r="AC2" s="261"/>
-      <c r="AD2" s="261"/>
-      <c r="AE2" s="261"/>
+      <c r="AB2" s="257"/>
+      <c r="AC2" s="257"/>
+      <c r="AD2" s="257"/>
+      <c r="AE2" s="257"/>
       <c r="AF2" s="95"/>
       <c r="AG2" s="95"/>
       <c r="AH2" s="95"/>
       <c r="AI2" s="95"/>
-      <c r="AJ2" s="261" t="s">
+      <c r="AJ2" s="257" t="s">
         <v>104</v>
       </c>
-      <c r="AK2" s="261"/>
-      <c r="AL2" s="261"/>
-      <c r="AM2" s="261"/>
-      <c r="AN2" s="261"/>
-      <c r="AO2" s="261"/>
-      <c r="AP2" s="261"/>
-      <c r="AQ2" s="261"/>
-      <c r="AR2" s="261"/>
-      <c r="AS2" s="261"/>
-      <c r="AT2" s="261"/>
-      <c r="AU2" s="261"/>
-      <c r="AV2" s="261"/>
-      <c r="AW2" s="262"/>
-      <c r="AX2" s="250" t="s">
+      <c r="AK2" s="257"/>
+      <c r="AL2" s="257"/>
+      <c r="AM2" s="257"/>
+      <c r="AN2" s="257"/>
+      <c r="AO2" s="257"/>
+      <c r="AP2" s="257"/>
+      <c r="AQ2" s="257"/>
+      <c r="AR2" s="257"/>
+      <c r="AS2" s="257"/>
+      <c r="AT2" s="257"/>
+      <c r="AU2" s="257"/>
+      <c r="AV2" s="257"/>
+      <c r="AW2" s="258"/>
+      <c r="AX2" s="246" t="s">
         <v>102</v>
       </c>
-      <c r="AY2" s="251"/>
-      <c r="AZ2" s="251"/>
-      <c r="BA2" s="251"/>
-      <c r="BB2" s="251"/>
-      <c r="BC2" s="251"/>
-      <c r="BD2" s="251"/>
-      <c r="BE2" s="251"/>
-      <c r="BF2" s="251"/>
-      <c r="BG2" s="251"/>
-      <c r="BH2" s="252"/>
+      <c r="AY2" s="247"/>
+      <c r="AZ2" s="247"/>
+      <c r="BA2" s="247"/>
+      <c r="BB2" s="247"/>
+      <c r="BC2" s="247"/>
+      <c r="BD2" s="247"/>
+      <c r="BE2" s="247"/>
+      <c r="BF2" s="247"/>
+      <c r="BG2" s="247"/>
+      <c r="BH2" s="248"/>
     </row>
     <row r="3" spans="1:60" s="7" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="259"/>
-      <c r="B3" s="260"/>
+      <c r="A3" s="255"/>
+      <c r="B3" s="256"/>
       <c r="C3" s="131" t="s">
         <v>0</v>
       </c>
@@ -8867,22 +8878,22 @@
       <c r="AD3" s="159" t="s">
         <v>87</v>
       </c>
-      <c r="AE3" s="184" t="s">
+      <c r="AE3" s="182" t="s">
         <v>89</v>
       </c>
       <c r="AF3" s="159" t="s">
         <v>90</v>
       </c>
-      <c r="AG3" s="201" t="s">
+      <c r="AG3" s="198" t="s">
         <v>91</v>
       </c>
-      <c r="AH3" s="201" t="s">
+      <c r="AH3" s="198" t="s">
         <v>92</v>
       </c>
-      <c r="AI3" s="206" t="s">
+      <c r="AI3" s="202" t="s">
         <v>94</v>
       </c>
-      <c r="AJ3" s="181" t="s">
+      <c r="AJ3" s="180" t="s">
         <v>0</v>
       </c>
       <c r="AK3" s="132" t="s">
@@ -8939,22 +8950,22 @@
       <c r="BB3" s="133" t="s">
         <v>89</v>
       </c>
-      <c r="BC3" s="190" t="s">
+      <c r="BC3" s="187" t="s">
         <v>90</v>
       </c>
-      <c r="BD3" s="190" t="s">
+      <c r="BD3" s="187" t="s">
         <v>91</v>
       </c>
-      <c r="BE3" s="190" t="s">
+      <c r="BE3" s="187" t="s">
         <v>92</v>
       </c>
-      <c r="BF3" s="190" t="s">
+      <c r="BF3" s="187" t="s">
         <v>94</v>
       </c>
-      <c r="BG3" s="191" t="s">
+      <c r="BG3" s="188" t="s">
         <v>103</v>
       </c>
-      <c r="BH3" s="192" t="s">
+      <c r="BH3" s="189" t="s">
         <v>105</v>
       </c>
     </row>
@@ -9049,19 +9060,19 @@
       <c r="AD4" s="157">
         <v>7.1428571428571432</v>
       </c>
-      <c r="AE4" s="185">
+      <c r="AE4" s="183">
         <v>7.1428571428571432</v>
       </c>
-      <c r="AF4" s="203">
+      <c r="AF4" s="200">
         <v>7.0588235294117636</v>
       </c>
-      <c r="AG4" s="182">
+      <c r="AG4" s="181">
         <v>7.3529411764705879</v>
       </c>
-      <c r="AH4" s="182">
+      <c r="AH4" s="181">
         <v>7.333333333333333</v>
       </c>
-      <c r="AI4" s="207">
+      <c r="AI4" s="203">
         <v>7.3170731707317076</v>
       </c>
       <c r="AJ4" s="155">
@@ -9140,27 +9151,27 @@
         <f t="shared" ref="BB4:BB15" si="7">+AE4/AD4-1</f>
         <v>0</v>
       </c>
-      <c r="BC4" s="193">
+      <c r="BC4" s="190">
         <f t="shared" ref="BC4:BC15" si="8">+AF4/AE4-1</f>
         <v>-1.1764705882353121E-2</v>
       </c>
-      <c r="BD4" s="193">
+      <c r="BD4" s="190">
         <f t="shared" ref="BD4:BD15" si="9">+AG4/AF4-1</f>
         <v>4.1666666666666741E-2</v>
       </c>
-      <c r="BE4" s="193">
+      <c r="BE4" s="190">
         <f t="shared" ref="BE4:BE15" si="10">+AH4/AG4-1</f>
         <v>-2.666666666666706E-3</v>
       </c>
-      <c r="BF4" s="193">
+      <c r="BF4" s="190">
         <f t="shared" ref="BF4:BF15" si="11">+AI4/AH4-1</f>
         <v>-2.2172949002216003E-3</v>
       </c>
-      <c r="BG4" s="193">
+      <c r="BG4" s="190">
         <f>+AI4/Z4-1</f>
         <v>-0.14634146341463405</v>
       </c>
-      <c r="BH4" s="194">
+      <c r="BH4" s="191">
         <f>+AI4/W4-1</f>
         <v>-0.12195121951219512</v>
       </c>
@@ -9256,7 +9267,7 @@
       <c r="AD5" s="152">
         <v>5.7142857142857144</v>
       </c>
-      <c r="AE5" s="186">
+      <c r="AE5" s="184">
         <v>5.833333333333333</v>
       </c>
       <c r="AF5" s="152">
@@ -9268,7 +9279,7 @@
       <c r="AH5" s="153">
         <v>5.833333333333333</v>
       </c>
-      <c r="AI5" s="208">
+      <c r="AI5" s="204">
         <v>5.4616477272727266</v>
       </c>
       <c r="AJ5" s="154">
@@ -9347,27 +9358,27 @@
         <f t="shared" si="7"/>
         <v>2.0833333333333259E-2</v>
       </c>
-      <c r="BC5" s="193">
+      <c r="BC5" s="190">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="BD5" s="193">
+      <c r="BD5" s="190">
         <f t="shared" si="9"/>
         <v>-3.2258064516128893E-2</v>
       </c>
-      <c r="BE5" s="193">
+      <c r="BE5" s="190">
         <f t="shared" si="10"/>
         <v>3.3333333333333215E-2</v>
       </c>
-      <c r="BF5" s="193">
+      <c r="BF5" s="190">
         <f t="shared" si="11"/>
         <v>-6.3717532467532534E-2</v>
       </c>
-      <c r="BG5" s="193">
+      <c r="BG5" s="190">
         <f t="shared" ref="BG5:BG14" si="12">+AI5/Z5-1</f>
         <v>-3.8395491425410433E-2</v>
       </c>
-      <c r="BH5" s="194">
+      <c r="BH5" s="191">
         <f t="shared" ref="BH5:BH14" si="13">+AI5/W5-1</f>
         <v>-6.3717532467532534E-2</v>
       </c>
@@ -9463,19 +9474,19 @@
       <c r="AD6" s="160">
         <v>10.90909090909091</v>
       </c>
-      <c r="AE6" s="187">
+      <c r="AE6" s="185">
         <v>11.111111111111111</v>
       </c>
       <c r="AF6" s="160">
         <v>10.83333333333333</v>
       </c>
-      <c r="AG6" s="162">
+      <c r="AG6" s="161">
         <v>10.83333333333333</v>
       </c>
-      <c r="AH6" s="162">
+      <c r="AH6" s="161">
         <v>10.8</v>
       </c>
-      <c r="AI6" s="209">
+      <c r="AI6" s="205">
         <v>10.82792207792208</v>
       </c>
       <c r="AJ6" s="154">
@@ -9554,27 +9565,27 @@
         <f t="shared" si="7"/>
         <v>1.8518518518518379E-2</v>
       </c>
-      <c r="BC6" s="193">
+      <c r="BC6" s="190">
         <f t="shared" si="8"/>
         <v>-2.5000000000000244E-2</v>
       </c>
-      <c r="BD6" s="193">
+      <c r="BD6" s="190">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="BE6" s="193">
+      <c r="BE6" s="190">
         <f t="shared" si="10"/>
         <v>-3.0769230769227551E-3</v>
       </c>
-      <c r="BF6" s="193">
+      <c r="BF6" s="190">
         <f t="shared" si="11"/>
         <v>2.5853775853776906E-3</v>
       </c>
-      <c r="BG6" s="193">
+      <c r="BG6" s="190">
         <f t="shared" si="12"/>
         <v>-5.2556818181818121E-2</v>
       </c>
-      <c r="BH6" s="194">
+      <c r="BH6" s="191">
         <f t="shared" si="13"/>
         <v>-2.5487012987012725E-2</v>
       </c>
@@ -9670,19 +9681,19 @@
       <c r="AD7" s="160">
         <v>9.2307692307692299</v>
       </c>
-      <c r="AE7" s="187">
+      <c r="AE7" s="185">
         <v>9.3023255813953494</v>
       </c>
       <c r="AF7" s="160">
         <v>8.75</v>
       </c>
-      <c r="AG7" s="162">
+      <c r="AG7" s="161">
         <v>9.0909090909090917</v>
       </c>
-      <c r="AH7" s="162">
+      <c r="AH7" s="161">
         <v>9.2307692307692299</v>
       </c>
-      <c r="AI7" s="209">
+      <c r="AI7" s="205">
         <v>9.2307692307692299</v>
       </c>
       <c r="AJ7" s="154">
@@ -9761,27 +9772,27 @@
         <f t="shared" si="7"/>
         <v>7.7519379844963598E-3</v>
       </c>
-      <c r="BC7" s="193">
+      <c r="BC7" s="190">
         <f t="shared" si="8"/>
         <v>-5.9375000000000067E-2</v>
       </c>
-      <c r="BD7" s="193">
+      <c r="BD7" s="190">
         <f t="shared" si="9"/>
         <v>3.8961038961039085E-2</v>
       </c>
-      <c r="BE7" s="193">
+      <c r="BE7" s="190">
         <f t="shared" si="10"/>
         <v>1.5384615384615108E-2</v>
       </c>
-      <c r="BF7" s="193">
+      <c r="BF7" s="190">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="BG7" s="193">
+      <c r="BG7" s="190">
         <f t="shared" si="12"/>
         <v>-0.12307692307692275</v>
       </c>
-      <c r="BH7" s="194">
+      <c r="BH7" s="191">
         <f t="shared" si="13"/>
         <v>-7.6923076923076983E-2</v>
       </c>
@@ -9877,19 +9888,19 @@
       <c r="AD8" s="160">
         <v>6.25</v>
       </c>
-      <c r="AE8" s="187">
+      <c r="AE8" s="185">
         <v>6.25</v>
       </c>
       <c r="AF8" s="160">
         <v>6.4102564102564106</v>
       </c>
-      <c r="AG8" s="162">
+      <c r="AG8" s="161">
         <v>6.25</v>
       </c>
-      <c r="AH8" s="162">
+      <c r="AH8" s="161">
         <v>6.4028026237328568</v>
       </c>
-      <c r="AI8" s="209">
+      <c r="AI8" s="205">
         <v>6.4516129032258061</v>
       </c>
       <c r="AJ8" s="154">
@@ -9968,27 +9979,27 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BC8" s="193">
+      <c r="BC8" s="190">
         <f t="shared" si="8"/>
         <v>2.5641025641025772E-2</v>
       </c>
-      <c r="BD8" s="193">
+      <c r="BD8" s="190">
         <f t="shared" si="9"/>
         <v>-2.5000000000000022E-2</v>
       </c>
-      <c r="BE8" s="193">
+      <c r="BE8" s="190">
         <f t="shared" si="10"/>
         <v>2.4448419797256982E-2</v>
       </c>
-      <c r="BF8" s="193">
+      <c r="BF8" s="190">
         <f t="shared" si="11"/>
         <v>7.623267865860317E-3</v>
       </c>
-      <c r="BG8" s="193">
+      <c r="BG8" s="190">
         <f t="shared" si="12"/>
         <v>-6.8100358422939156E-2</v>
       </c>
-      <c r="BH8" s="194">
+      <c r="BH8" s="191">
         <f t="shared" si="13"/>
         <v>-9.1322126306224494E-2</v>
       </c>
@@ -10084,19 +10095,19 @@
       <c r="AD9" s="160">
         <v>7.291666666666667</v>
       </c>
-      <c r="AE9" s="187">
+      <c r="AE9" s="185">
         <v>7.291666666666667</v>
       </c>
       <c r="AF9" s="160">
         <v>7.6923076923076934</v>
       </c>
-      <c r="AG9" s="162">
+      <c r="AG9" s="161">
         <v>7.0370370370370372</v>
       </c>
-      <c r="AH9" s="162">
+      <c r="AH9" s="161">
         <v>7.372837297383775</v>
       </c>
-      <c r="AI9" s="209">
+      <c r="AI9" s="205">
         <v>7.2727272727272716</v>
       </c>
       <c r="AJ9" s="154">
@@ -10175,27 +10186,27 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BC9" s="193">
+      <c r="BC9" s="190">
         <f t="shared" si="8"/>
         <v>5.4945054945054972E-2</v>
       </c>
-      <c r="BD9" s="193">
+      <c r="BD9" s="190">
         <f t="shared" si="9"/>
         <v>-8.5185185185185253E-2</v>
       </c>
-      <c r="BE9" s="193">
+      <c r="BE9" s="190">
         <f t="shared" si="10"/>
         <v>4.7718984365062722E-2</v>
       </c>
-      <c r="BF9" s="193">
+      <c r="BF9" s="190">
         <f t="shared" si="11"/>
         <v>-1.3578222415409513E-2</v>
       </c>
-      <c r="BG9" s="193">
+      <c r="BG9" s="190">
         <f t="shared" si="12"/>
         <v>-7.4380165289256284E-2</v>
       </c>
-      <c r="BH9" s="194">
+      <c r="BH9" s="191">
         <f t="shared" si="13"/>
         <v>-1.7199017199017397E-2</v>
       </c>
@@ -10291,19 +10302,19 @@
       <c r="AD10" s="160">
         <v>8</v>
       </c>
-      <c r="AE10" s="187">
+      <c r="AE10" s="185">
         <v>8.0825791855203626</v>
       </c>
       <c r="AF10" s="160">
         <v>8</v>
       </c>
-      <c r="AG10" s="162">
+      <c r="AG10" s="161">
         <v>8</v>
       </c>
-      <c r="AH10" s="162">
+      <c r="AH10" s="161">
         <v>8</v>
       </c>
-      <c r="AI10" s="209">
+      <c r="AI10" s="205">
         <v>8</v>
       </c>
       <c r="AJ10" s="154">
@@ -10382,27 +10393,27 @@
         <f t="shared" si="7"/>
         <v>1.0322398190045323E-2</v>
       </c>
-      <c r="BC10" s="193">
+      <c r="BC10" s="190">
         <f t="shared" si="8"/>
         <v>-1.0216934919524245E-2</v>
       </c>
-      <c r="BD10" s="193">
+      <c r="BD10" s="190">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="BE10" s="193">
+      <c r="BE10" s="190">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="BF10" s="193">
+      <c r="BF10" s="190">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="BG10" s="193">
+      <c r="BG10" s="190">
         <f t="shared" si="12"/>
         <v>-0.1272727272727272</v>
       </c>
-      <c r="BH10" s="194">
+      <c r="BH10" s="191">
         <f t="shared" si="13"/>
         <v>-8.5714285714285743E-2</v>
       </c>
@@ -10498,19 +10509,19 @@
       <c r="AD11" s="160">
         <v>10.52631578947368</v>
       </c>
-      <c r="AE11" s="187">
+      <c r="AE11" s="185">
         <v>10.52631578947368</v>
       </c>
       <c r="AF11" s="160">
         <v>10</v>
       </c>
-      <c r="AG11" s="162">
+      <c r="AG11" s="161">
         <v>10.4</v>
       </c>
-      <c r="AH11" s="162">
+      <c r="AH11" s="161">
         <v>10</v>
       </c>
-      <c r="AI11" s="209">
+      <c r="AI11" s="205">
         <v>10.71428571428571</v>
       </c>
       <c r="AJ11" s="154">
@@ -10589,27 +10600,27 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BC11" s="193">
+      <c r="BC11" s="190">
         <f t="shared" si="8"/>
         <v>-4.99999999999996E-2</v>
       </c>
-      <c r="BD11" s="193">
+      <c r="BD11" s="190">
         <f t="shared" si="9"/>
         <v>4.0000000000000036E-2</v>
       </c>
-      <c r="BE11" s="193">
+      <c r="BE11" s="190">
         <f t="shared" si="10"/>
         <v>-3.8461538461538547E-2</v>
       </c>
-      <c r="BF11" s="193">
+      <c r="BF11" s="190">
         <f t="shared" si="11"/>
         <v>7.1428571428570953E-2</v>
       </c>
-      <c r="BG11" s="193">
+      <c r="BG11" s="190">
         <f t="shared" si="12"/>
         <v>-9.3406593406593963E-2</v>
       </c>
-      <c r="BH11" s="194">
+      <c r="BH11" s="191">
         <f t="shared" si="13"/>
         <v>-5.1833122629583284E-2</v>
       </c>
@@ -10705,19 +10716,19 @@
       <c r="AD12" s="160">
         <v>8.5714285714285712</v>
       </c>
-      <c r="AE12" s="187">
+      <c r="AE12" s="185">
         <v>8.6956521739130395</v>
       </c>
       <c r="AF12" s="160">
         <v>8.4210526315789469</v>
       </c>
-      <c r="AG12" s="162">
+      <c r="AG12" s="161">
         <v>8.1818181818181817</v>
       </c>
-      <c r="AH12" s="162">
+      <c r="AH12" s="161">
         <v>8.3333333333333339</v>
       </c>
-      <c r="AI12" s="209">
+      <c r="AI12" s="205">
         <v>8.3333333333333339</v>
       </c>
       <c r="AJ12" s="154">
@@ -10796,27 +10807,27 @@
         <f t="shared" si="7"/>
         <v>1.4492753623188026E-2</v>
       </c>
-      <c r="BC12" s="193">
+      <c r="BC12" s="190">
         <f t="shared" si="8"/>
         <v>-3.1578947368420707E-2</v>
       </c>
-      <c r="BD12" s="193">
+      <c r="BD12" s="190">
         <f t="shared" si="9"/>
         <v>-2.8409090909090828E-2</v>
       </c>
-      <c r="BE12" s="193">
+      <c r="BE12" s="190">
         <f t="shared" si="10"/>
         <v>1.8518518518518601E-2</v>
       </c>
-      <c r="BF12" s="193">
+      <c r="BF12" s="190">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="BG12" s="193">
+      <c r="BG12" s="190">
         <f t="shared" si="12"/>
         <v>-0.11904761904761896</v>
       </c>
-      <c r="BH12" s="194">
+      <c r="BH12" s="191">
         <f t="shared" si="13"/>
         <v>-8.013937282229977E-2</v>
       </c>
@@ -10912,19 +10923,19 @@
       <c r="AD13" s="160">
         <v>10</v>
       </c>
-      <c r="AE13" s="187">
+      <c r="AE13" s="185">
         <v>10</v>
       </c>
       <c r="AF13" s="160">
         <v>10</v>
       </c>
-      <c r="AG13" s="162">
+      <c r="AG13" s="161">
         <v>10</v>
       </c>
-      <c r="AH13" s="162">
+      <c r="AH13" s="161">
         <v>9.375</v>
       </c>
-      <c r="AI13" s="209">
+      <c r="AI13" s="205">
         <v>10</v>
       </c>
       <c r="AJ13" s="154">
@@ -11003,27 +11014,27 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BC13" s="193">
+      <c r="BC13" s="190">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="BD13" s="193">
+      <c r="BD13" s="190">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="BE13" s="193">
+      <c r="BE13" s="190">
         <f t="shared" si="10"/>
         <v>-6.25E-2</v>
       </c>
-      <c r="BF13" s="193">
+      <c r="BF13" s="190">
         <f t="shared" si="11"/>
         <v>6.6666666666666652E-2</v>
       </c>
-      <c r="BG13" s="193">
+      <c r="BG13" s="190">
         <f t="shared" si="12"/>
         <v>-7.1428571428571508E-2</v>
       </c>
-      <c r="BH13" s="194">
+      <c r="BH13" s="191">
         <f t="shared" si="13"/>
         <v>-0.11111111111111116</v>
       </c>
@@ -11119,7 +11130,7 @@
       <c r="AD14" s="144">
         <v>7.8571428571428568</v>
       </c>
-      <c r="AE14" s="188">
+      <c r="AE14" s="186">
         <v>8.085106382978724</v>
       </c>
       <c r="AF14" s="144">
@@ -11131,7 +11142,7 @@
       <c r="AH14" s="158">
         <v>8.0882352941176467</v>
       </c>
-      <c r="AI14" s="210">
+      <c r="AI14" s="206">
         <v>8.0882352941176467</v>
       </c>
       <c r="AJ14" s="156">
@@ -11210,36 +11221,36 @@
         <f t="shared" si="7"/>
         <v>2.9013539651837617E-2</v>
       </c>
-      <c r="BC14" s="193">
+      <c r="BC14" s="190">
         <f t="shared" si="8"/>
         <v>-1.0526315789473717E-2</v>
       </c>
-      <c r="BD14" s="193">
+      <c r="BD14" s="190">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="BE14" s="193">
+      <c r="BE14" s="190">
         <f t="shared" si="10"/>
         <v>1.1029411764705843E-2</v>
       </c>
-      <c r="BF14" s="193">
+      <c r="BF14" s="190">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="BG14" s="193">
+      <c r="BG14" s="190">
         <f t="shared" si="12"/>
         <v>-0.14359861591695511</v>
       </c>
-      <c r="BH14" s="194">
+      <c r="BH14" s="191">
         <f t="shared" si="13"/>
         <v>-0.16176470588235303</v>
       </c>
     </row>
     <row r="15" spans="1:60" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="231" t="s">
+      <c r="A15" s="227" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="233"/>
+      <c r="B15" s="229"/>
       <c r="C15" s="47">
         <f>AVERAGE(C4:C14)</f>
         <v>8.0843345048625608</v>
@@ -11332,24 +11343,24 @@
       <c r="AC15" s="129">
         <v>8.6999999999999993</v>
       </c>
-      <c r="AD15" s="161">
+      <c r="AD15" s="260">
         <v>8.3000000000000007</v>
       </c>
-      <c r="AE15" s="189">
+      <c r="AE15" s="261">
         <v>8.4</v>
       </c>
-      <c r="AF15" s="204">
+      <c r="AF15" s="262">
         <v>8.3000000000000007</v>
       </c>
-      <c r="AG15" s="183">
+      <c r="AG15" s="263">
         <f>+AVERAGE(AG4:AG14)</f>
         <v>8.2537454645355286</v>
       </c>
-      <c r="AH15" s="183">
+      <c r="AH15" s="263">
         <f>+AVERAGE(AH4:AH14)</f>
         <v>8.2517858587275921</v>
       </c>
-      <c r="AI15" s="183">
+      <c r="AI15" s="263">
         <f>+AVERAGE(AI4:AI14)</f>
         <v>8.3361460658532298</v>
       </c>
@@ -11429,27 +11440,27 @@
         <f t="shared" si="7"/>
         <v>1.2048192771084265E-2</v>
       </c>
-      <c r="BC15" s="195">
+      <c r="BC15" s="192">
         <f t="shared" si="8"/>
         <v>-1.1904761904761862E-2</v>
       </c>
-      <c r="BD15" s="195">
+      <c r="BD15" s="192">
         <f t="shared" si="9"/>
         <v>-5.5728355981291555E-3</v>
       </c>
-      <c r="BE15" s="195">
+      <c r="BE15" s="192">
         <f t="shared" si="10"/>
         <v>-2.374201889744354E-4</v>
       </c>
-      <c r="BF15" s="195">
+      <c r="BF15" s="192">
         <f t="shared" si="11"/>
         <v>1.0223266644324491E-2</v>
       </c>
-      <c r="BG15" s="195">
+      <c r="BG15" s="192">
         <f>+AI15/Z15-1</f>
         <v>-9.3897166755083639E-2</v>
       </c>
-      <c r="BH15" s="196">
+      <c r="BH15" s="193">
         <f>+AI15/W15-1</f>
         <v>-8.3939992763381266E-2</v>
       </c>
@@ -11465,6 +11476,18 @@
     <mergeCell ref="AA2:AE2"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
+  <conditionalFormatting sqref="BH4:BH15">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>